<commit_message>
Extract text from minutes (pdf), first version
</commit_message>
<xml_diff>
--- a/minutes_format.xlsx
+++ b/minutes_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatheusBreitenbach\Documents\VSCode_Projects\0 - TCC\br-central-bank-sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC65C253-459F-43C4-BED8-006CAF486736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE096B7-8295-4FFF-B8AB-49D7E49BD6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="234">
   <si>
     <t>Titulo</t>
   </si>
@@ -738,6 +738,9 @@
   </si>
   <si>
     <t>InitialPage</t>
+  </si>
+  <si>
+    <t>NeedAdjust</t>
   </si>
 </sst>
 </file>
@@ -769,7 +772,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -806,6 +809,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -834,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -870,6 +879,12 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1151,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D230"/>
+  <dimension ref="A1:E230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A231" sqref="A231:XFD231"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,9 +1178,10 @@
     <col min="2" max="2" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1178,8 +1194,11 @@
       <c r="D1" s="7" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>229</v>
       </c>
@@ -1192,12 +1211,15 @@
       <c r="D2" s="14">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="16">
         <v>1</v>
       </c>
       <c r="C3" s="8">
@@ -1206,12 +1228,15 @@
       <c r="D3" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="16">
         <v>1</v>
       </c>
       <c r="C4" s="8">
@@ -1220,12 +1245,15 @@
       <c r="D4" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="16">
         <v>1</v>
       </c>
       <c r="C5" s="8">
@@ -1234,12 +1262,15 @@
       <c r="D5" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="16">
         <v>1</v>
       </c>
       <c r="C6" s="8">
@@ -1248,12 +1279,15 @@
       <c r="D6" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="16">
         <v>1</v>
       </c>
       <c r="C7" s="8">
@@ -1262,12 +1296,15 @@
       <c r="D7" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="16">
         <v>1</v>
       </c>
       <c r="C8" s="8">
@@ -1276,8 +1313,11 @@
       <c r="D8" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>222</v>
       </c>
@@ -1290,8 +1330,11 @@
       <c r="D9" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>221</v>
       </c>
@@ -1304,8 +1347,11 @@
       <c r="D10" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>220</v>
       </c>
@@ -1318,8 +1364,11 @@
       <c r="D11" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>219</v>
       </c>
@@ -1332,8 +1381,11 @@
       <c r="D12" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>218</v>
       </c>
@@ -1346,8 +1398,11 @@
       <c r="D13" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>217</v>
       </c>
@@ -1360,8 +1415,11 @@
       <c r="D14" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>216</v>
       </c>
@@ -1374,8 +1432,11 @@
       <c r="D15" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>215</v>
       </c>
@@ -1388,8 +1449,11 @@
       <c r="D16" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>214</v>
       </c>
@@ -1402,8 +1466,11 @@
       <c r="D17" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>213</v>
       </c>
@@ -1416,8 +1483,11 @@
       <c r="D18" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>212</v>
       </c>
@@ -1430,12 +1500,15 @@
       <c r="D19" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="16">
         <v>2</v>
       </c>
       <c r="C20" s="9">
@@ -1444,8 +1517,11 @@
       <c r="D20" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>210</v>
       </c>
@@ -1458,8 +1534,11 @@
       <c r="D21" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>209</v>
       </c>
@@ -1472,8 +1551,11 @@
       <c r="D22" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>208</v>
       </c>
@@ -1486,8 +1568,11 @@
       <c r="D23" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>207</v>
       </c>
@@ -1500,8 +1585,11 @@
       <c r="D24" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>206</v>
       </c>
@@ -1514,8 +1602,11 @@
       <c r="D25" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>205</v>
       </c>
@@ -1528,8 +1619,11 @@
       <c r="D26" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>204</v>
       </c>
@@ -1542,8 +1636,11 @@
       <c r="D27" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>203</v>
       </c>
@@ -1556,8 +1653,11 @@
       <c r="D28" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>202</v>
       </c>
@@ -1570,8 +1670,11 @@
       <c r="D29" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>201</v>
       </c>
@@ -1584,8 +1687,11 @@
       <c r="D30" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>200</v>
       </c>
@@ -1598,8 +1704,11 @@
       <c r="D31" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>199</v>
       </c>
@@ -1612,8 +1721,11 @@
       <c r="D32" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>198</v>
       </c>
@@ -1626,8 +1738,11 @@
       <c r="D33" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>197</v>
       </c>
@@ -1640,8 +1755,11 @@
       <c r="D34" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>196</v>
       </c>
@@ -1654,8 +1772,11 @@
       <c r="D35" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>195</v>
       </c>
@@ -1668,8 +1789,11 @@
       <c r="D36" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>194</v>
       </c>
@@ -1682,8 +1806,11 @@
       <c r="D37" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>193</v>
       </c>
@@ -1696,8 +1823,11 @@
       <c r="D38" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>192</v>
       </c>
@@ -1710,8 +1840,11 @@
       <c r="D39" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>191</v>
       </c>
@@ -1724,8 +1857,11 @@
       <c r="D40" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>190</v>
       </c>
@@ -1738,8 +1874,11 @@
       <c r="D41" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>189</v>
       </c>
@@ -1752,8 +1891,11 @@
       <c r="D42" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>188</v>
       </c>
@@ -1766,8 +1908,11 @@
       <c r="D43" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>187</v>
       </c>
@@ -1780,8 +1925,11 @@
       <c r="D44" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>186</v>
       </c>
@@ -1794,8 +1942,11 @@
       <c r="D45" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>185</v>
       </c>
@@ -1808,8 +1959,11 @@
       <c r="D46" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>184</v>
       </c>
@@ -1822,8 +1976,11 @@
       <c r="D47" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>183</v>
       </c>
@@ -1836,8 +1993,11 @@
       <c r="D48" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>182</v>
       </c>
@@ -1850,8 +2010,11 @@
       <c r="D49" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>181</v>
       </c>
@@ -1864,8 +2027,11 @@
       <c r="D50" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>180</v>
       </c>
@@ -1878,8 +2044,11 @@
       <c r="D51" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>179</v>
       </c>
@@ -1892,8 +2061,11 @@
       <c r="D52" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>178</v>
       </c>
@@ -1906,8 +2078,11 @@
       <c r="D53" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>177</v>
       </c>
@@ -1920,8 +2095,11 @@
       <c r="D54" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>176</v>
       </c>
@@ -1934,8 +2112,11 @@
       <c r="D55" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>175</v>
       </c>
@@ -1948,8 +2129,11 @@
       <c r="D56" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>174</v>
       </c>
@@ -1962,8 +2146,11 @@
       <c r="D57" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>173</v>
       </c>
@@ -1976,8 +2163,11 @@
       <c r="D58" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>172</v>
       </c>
@@ -1990,8 +2180,11 @@
       <c r="D59" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>171</v>
       </c>
@@ -2004,8 +2197,11 @@
       <c r="D60" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>170</v>
       </c>
@@ -2018,8 +2214,11 @@
       <c r="D61" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>169</v>
       </c>
@@ -2032,8 +2231,11 @@
       <c r="D62" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>168</v>
       </c>
@@ -2046,8 +2248,11 @@
       <c r="D63" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>167</v>
       </c>
@@ -2060,8 +2265,11 @@
       <c r="D64" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>166</v>
       </c>
@@ -2074,8 +2282,11 @@
       <c r="D65" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>165</v>
       </c>
@@ -2088,8 +2299,11 @@
       <c r="D66" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>164</v>
       </c>
@@ -2102,8 +2316,11 @@
       <c r="D67" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>163</v>
       </c>
@@ -2116,8 +2333,11 @@
       <c r="D68" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>162</v>
       </c>
@@ -2130,8 +2350,11 @@
       <c r="D69" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>161</v>
       </c>
@@ -2144,8 +2367,11 @@
       <c r="D70" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>160</v>
       </c>
@@ -2158,8 +2384,11 @@
       <c r="D71" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>159</v>
       </c>
@@ -2172,8 +2401,11 @@
       <c r="D72" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>158</v>
       </c>
@@ -2186,8 +2418,11 @@
       <c r="D73" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>157</v>
       </c>
@@ -2200,8 +2435,11 @@
       <c r="D74" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>156</v>
       </c>
@@ -2214,8 +2452,11 @@
       <c r="D75" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>155</v>
       </c>
@@ -2228,8 +2469,11 @@
       <c r="D76" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>154</v>
       </c>
@@ -2242,8 +2486,11 @@
       <c r="D77" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>153</v>
       </c>
@@ -2256,8 +2503,11 @@
       <c r="D78" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>152</v>
       </c>
@@ -2270,8 +2520,11 @@
       <c r="D79" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>151</v>
       </c>
@@ -2284,8 +2537,11 @@
       <c r="D80" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>150</v>
       </c>
@@ -2298,8 +2554,11 @@
       <c r="D81" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>149</v>
       </c>
@@ -2312,8 +2571,11 @@
       <c r="D82" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>148</v>
       </c>
@@ -2326,8 +2588,11 @@
       <c r="D83" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>147</v>
       </c>
@@ -2340,8 +2605,11 @@
       <c r="D84" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>146</v>
       </c>
@@ -2354,8 +2622,11 @@
       <c r="D85" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>145</v>
       </c>
@@ -2368,8 +2639,11 @@
       <c r="D86" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>144</v>
       </c>
@@ -2382,8 +2656,11 @@
       <c r="D87" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>143</v>
       </c>
@@ -2396,8 +2673,11 @@
       <c r="D88" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>142</v>
       </c>
@@ -2410,8 +2690,11 @@
       <c r="D89" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>141</v>
       </c>
@@ -2424,8 +2707,11 @@
       <c r="D90" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>140</v>
       </c>
@@ -2438,8 +2724,11 @@
       <c r="D91" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>139</v>
       </c>
@@ -2452,8 +2741,11 @@
       <c r="D92" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>138</v>
       </c>
@@ -2466,8 +2758,11 @@
       <c r="D93" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>137</v>
       </c>
@@ -2480,8 +2775,11 @@
       <c r="D94" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>136</v>
       </c>
@@ -2494,8 +2792,11 @@
       <c r="D95" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>135</v>
       </c>
@@ -2508,8 +2809,11 @@
       <c r="D96" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>134</v>
       </c>
@@ -2522,8 +2826,11 @@
       <c r="D97" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>133</v>
       </c>
@@ -2536,8 +2843,11 @@
       <c r="D98" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>132</v>
       </c>
@@ -2550,8 +2860,11 @@
       <c r="D99" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>131</v>
       </c>
@@ -2564,8 +2877,11 @@
       <c r="D100" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>130</v>
       </c>
@@ -2578,8 +2894,11 @@
       <c r="D101" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>129</v>
       </c>
@@ -2592,8 +2911,11 @@
       <c r="D102" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>128</v>
       </c>
@@ -2606,8 +2928,11 @@
       <c r="D103" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>127</v>
       </c>
@@ -2620,8 +2945,11 @@
       <c r="D104" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>126</v>
       </c>
@@ -2634,8 +2962,11 @@
       <c r="D105" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>125</v>
       </c>
@@ -2648,8 +2979,11 @@
       <c r="D106" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>124</v>
       </c>
@@ -2662,8 +2996,11 @@
       <c r="D107" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>123</v>
       </c>
@@ -2676,8 +3013,11 @@
       <c r="D108" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>122</v>
       </c>
@@ -2690,8 +3030,11 @@
       <c r="D109" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>121</v>
       </c>
@@ -2704,8 +3047,11 @@
       <c r="D110" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>120</v>
       </c>
@@ -2718,8 +3064,11 @@
       <c r="D111" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>119</v>
       </c>
@@ -2732,8 +3081,11 @@
       <c r="D112" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>118</v>
       </c>
@@ -2746,8 +3098,11 @@
       <c r="D113" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>117</v>
       </c>
@@ -2760,8 +3115,11 @@
       <c r="D114" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>116</v>
       </c>
@@ -2774,8 +3132,11 @@
       <c r="D115" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>115</v>
       </c>
@@ -2788,8 +3149,11 @@
       <c r="D116" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>114</v>
       </c>
@@ -2802,8 +3166,11 @@
       <c r="D117" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>113</v>
       </c>
@@ -2816,8 +3183,11 @@
       <c r="D118" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>112</v>
       </c>
@@ -2830,8 +3200,11 @@
       <c r="D119" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>111</v>
       </c>
@@ -2844,8 +3217,11 @@
       <c r="D120" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>110</v>
       </c>
@@ -2858,8 +3234,11 @@
       <c r="D121" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>109</v>
       </c>
@@ -2872,8 +3251,11 @@
       <c r="D122" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>108</v>
       </c>
@@ -2886,8 +3268,11 @@
       <c r="D123" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>107</v>
       </c>
@@ -2900,8 +3285,11 @@
       <c r="D124" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>106</v>
       </c>
@@ -2914,8 +3302,11 @@
       <c r="D125" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>105</v>
       </c>
@@ -2928,8 +3319,11 @@
       <c r="D126" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>104</v>
       </c>
@@ -2942,8 +3336,11 @@
       <c r="D127" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>103</v>
       </c>
@@ -2956,8 +3353,11 @@
       <c r="D128" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>102</v>
       </c>
@@ -2970,8 +3370,11 @@
       <c r="D129" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>101</v>
       </c>
@@ -2984,8 +3387,11 @@
       <c r="D130" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>100</v>
       </c>
@@ -2998,8 +3404,11 @@
       <c r="D131" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>99</v>
       </c>
@@ -3012,8 +3421,11 @@
       <c r="D132" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>98</v>
       </c>
@@ -3026,8 +3438,11 @@
       <c r="D133" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>97</v>
       </c>
@@ -3040,8 +3455,11 @@
       <c r="D134" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>96</v>
       </c>
@@ -3054,8 +3472,11 @@
       <c r="D135" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>95</v>
       </c>
@@ -3068,8 +3489,11 @@
       <c r="D136" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>94</v>
       </c>
@@ -3082,8 +3506,11 @@
       <c r="D137" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>93</v>
       </c>
@@ -3096,8 +3523,11 @@
       <c r="D138" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>92</v>
       </c>
@@ -3110,8 +3540,11 @@
       <c r="D139" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>91</v>
       </c>
@@ -3124,8 +3557,11 @@
       <c r="D140" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>90</v>
       </c>
@@ -3138,8 +3574,11 @@
       <c r="D141" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>89</v>
       </c>
@@ -3152,8 +3591,11 @@
       <c r="D142" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>88</v>
       </c>
@@ -3166,8 +3608,11 @@
       <c r="D143" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>87</v>
       </c>
@@ -3180,8 +3625,11 @@
       <c r="D144" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>86</v>
       </c>
@@ -3194,8 +3642,11 @@
       <c r="D145" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>85</v>
       </c>
@@ -3208,8 +3659,11 @@
       <c r="D146" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>84</v>
       </c>
@@ -3222,8 +3676,11 @@
       <c r="D147" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>83</v>
       </c>
@@ -3236,8 +3693,11 @@
       <c r="D148" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>82</v>
       </c>
@@ -3250,8 +3710,11 @@
       <c r="D149" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>81</v>
       </c>
@@ -3264,8 +3727,11 @@
       <c r="D150" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>80</v>
       </c>
@@ -3278,8 +3744,11 @@
       <c r="D151" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>79</v>
       </c>
@@ -3292,8 +3761,11 @@
       <c r="D152" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>78</v>
       </c>
@@ -3306,8 +3778,11 @@
       <c r="D153" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>77</v>
       </c>
@@ -3320,8 +3795,11 @@
       <c r="D154" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>76</v>
       </c>
@@ -3334,8 +3812,11 @@
       <c r="D155" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>75</v>
       </c>
@@ -3348,8 +3829,11 @@
       <c r="D156" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>74</v>
       </c>
@@ -3362,8 +3846,11 @@
       <c r="D157" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>73</v>
       </c>
@@ -3376,8 +3863,11 @@
       <c r="D158" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>72</v>
       </c>
@@ -3390,8 +3880,11 @@
       <c r="D159" s="15">
         <v>4</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>71</v>
       </c>
@@ -3404,8 +3897,11 @@
       <c r="D160" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E160" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>70</v>
       </c>
@@ -3418,8 +3914,11 @@
       <c r="D161" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E161" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>69</v>
       </c>
@@ -3432,8 +3931,11 @@
       <c r="D162" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>68</v>
       </c>
@@ -3446,8 +3948,11 @@
       <c r="D163" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E163" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>67</v>
       </c>
@@ -3460,8 +3965,11 @@
       <c r="D164" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E164" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>66</v>
       </c>
@@ -3474,8 +3982,11 @@
       <c r="D165" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E165" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>65</v>
       </c>
@@ -3488,8 +3999,11 @@
       <c r="D166" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>64</v>
       </c>
@@ -3502,8 +4016,11 @@
       <c r="D167" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>63</v>
       </c>
@@ -3516,8 +4033,11 @@
       <c r="D168" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>62</v>
       </c>
@@ -3530,8 +4050,11 @@
       <c r="D169" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E169" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>61</v>
       </c>
@@ -3544,8 +4067,11 @@
       <c r="D170" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E170" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>60</v>
       </c>
@@ -3558,8 +4084,11 @@
       <c r="D171" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E171" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>59</v>
       </c>
@@ -3572,8 +4101,11 @@
       <c r="D172" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>58</v>
       </c>
@@ -3586,8 +4118,11 @@
       <c r="D173" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E173" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>57</v>
       </c>
@@ -3600,8 +4135,11 @@
       <c r="D174" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E174" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>56</v>
       </c>
@@ -3614,8 +4152,11 @@
       <c r="D175" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E175" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>55</v>
       </c>
@@ -3628,8 +4169,11 @@
       <c r="D176" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>54</v>
       </c>
@@ -3642,8 +4186,11 @@
       <c r="D177" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>53</v>
       </c>
@@ -3656,8 +4203,11 @@
       <c r="D178" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>52</v>
       </c>
@@ -3670,8 +4220,11 @@
       <c r="D179" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>51</v>
       </c>
@@ -3684,8 +4237,11 @@
       <c r="D180" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E180" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>50</v>
       </c>
@@ -3698,8 +4254,11 @@
       <c r="D181" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>49</v>
       </c>
@@ -3712,8 +4271,11 @@
       <c r="D182" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E182" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>48</v>
       </c>
@@ -3726,8 +4288,11 @@
       <c r="D183" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E183" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>47</v>
       </c>
@@ -3740,8 +4305,11 @@
       <c r="D184" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>46</v>
       </c>
@@ -3754,8 +4322,11 @@
       <c r="D185" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>45</v>
       </c>
@@ -3768,8 +4339,11 @@
       <c r="D186" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E186" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>44</v>
       </c>
@@ -3782,8 +4356,11 @@
       <c r="D187" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>43</v>
       </c>
@@ -3796,8 +4373,11 @@
       <c r="D188" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E188" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>42</v>
       </c>
@@ -3810,8 +4390,11 @@
       <c r="D189" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E189" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>41</v>
       </c>
@@ -3824,8 +4407,11 @@
       <c r="D190" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E190" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>40</v>
       </c>
@@ -3838,8 +4424,11 @@
       <c r="D191" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E191" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>39</v>
       </c>
@@ -3852,8 +4441,11 @@
       <c r="D192" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>38</v>
       </c>
@@ -3866,8 +4458,11 @@
       <c r="D193" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E193" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>37</v>
       </c>
@@ -3880,8 +4475,11 @@
       <c r="D194" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E194" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>36</v>
       </c>
@@ -3894,8 +4492,11 @@
       <c r="D195" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E195" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>35</v>
       </c>
@@ -3908,8 +4509,11 @@
       <c r="D196" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E196" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>34</v>
       </c>
@@ -3922,8 +4526,11 @@
       <c r="D197" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E197" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>33</v>
       </c>
@@ -3936,8 +4543,11 @@
       <c r="D198" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E198" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>32</v>
       </c>
@@ -3950,8 +4560,11 @@
       <c r="D199" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E199" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>31</v>
       </c>
@@ -3964,8 +4577,11 @@
       <c r="D200" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E200" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>30</v>
       </c>
@@ -3978,8 +4594,11 @@
       <c r="D201" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E201" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>29</v>
       </c>
@@ -3992,8 +4611,11 @@
       <c r="D202" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E202" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>28</v>
       </c>
@@ -4006,8 +4628,11 @@
       <c r="D203" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E203" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>27</v>
       </c>
@@ -4020,8 +4645,11 @@
       <c r="D204" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E204" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>26</v>
       </c>
@@ -4034,8 +4662,11 @@
       <c r="D205" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E205" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>25</v>
       </c>
@@ -4048,8 +4679,11 @@
       <c r="D206" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E206" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>24</v>
       </c>
@@ -4062,8 +4696,11 @@
       <c r="D207" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E207" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>23</v>
       </c>
@@ -4076,8 +4713,11 @@
       <c r="D208" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E208" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>22</v>
       </c>
@@ -4090,8 +4730,11 @@
       <c r="D209" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>21</v>
       </c>
@@ -4104,8 +4747,11 @@
       <c r="D210" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>20</v>
       </c>
@@ -4118,8 +4764,11 @@
       <c r="D211" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>19</v>
       </c>
@@ -4132,8 +4781,11 @@
       <c r="D212" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E212" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>18</v>
       </c>
@@ -4146,8 +4798,11 @@
       <c r="D213" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>17</v>
       </c>
@@ -4160,8 +4815,11 @@
       <c r="D214" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E214" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>16</v>
       </c>
@@ -4174,8 +4832,11 @@
       <c r="D215" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>15</v>
       </c>
@@ -4188,8 +4849,11 @@
       <c r="D216" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E216" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>14</v>
       </c>
@@ -4202,8 +4866,11 @@
       <c r="D217" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E217" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>13</v>
       </c>
@@ -4216,8 +4883,11 @@
       <c r="D218" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E218" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>12</v>
       </c>
@@ -4230,8 +4900,11 @@
       <c r="D219" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E219" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>11</v>
       </c>
@@ -4244,8 +4917,11 @@
       <c r="D220" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E220" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>10</v>
       </c>
@@ -4258,8 +4934,11 @@
       <c r="D221" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E221" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>9</v>
       </c>
@@ -4272,8 +4951,11 @@
       <c r="D222" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E222" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>8</v>
       </c>
@@ -4286,8 +4968,11 @@
       <c r="D223" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E223" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>7</v>
       </c>
@@ -4300,8 +4985,11 @@
       <c r="D224" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>6</v>
       </c>
@@ -4314,8 +5002,11 @@
       <c r="D225" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E225" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>5</v>
       </c>
@@ -4328,8 +5019,11 @@
       <c r="D226" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E226" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>4</v>
       </c>
@@ -4342,8 +5036,11 @@
       <c r="D227" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E227" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>3</v>
       </c>
@@ -4356,8 +5053,11 @@
       <c r="D228" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E228" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>2</v>
       </c>
@@ -4370,8 +5070,11 @@
       <c r="D229" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E229" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>1</v>
       </c>
@@ -4383,6 +5086,9 @@
       </c>
       <c r="D230" s="12">
         <v>3</v>
+      </c>
+      <c r="E230" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust text format from auto extraction
</commit_message>
<xml_diff>
--- a/minutes_format.xlsx
+++ b/minutes_format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatheusBreitenbach\Documents\VSCode_Projects\0 - TCC\br-central-bank-sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE096B7-8295-4FFF-B8AB-49D7E49BD6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB34DCA-8A0E-49EB-B28E-796F345D267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -740,7 +740,7 @@
     <t>InitialPage</t>
   </si>
   <si>
-    <t>NeedAdjust</t>
+    <t>Ignore</t>
   </si>
 </sst>
 </file>
@@ -883,7 +883,7 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1169,7 +1169,7 @@
   <dimension ref="A1:E230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1212,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>